<commit_message>
Rearranged 07.xlsx and updated 02_diltuion.R
Toyed with converting OD600 to bacterial contribution. Will go back in to look at the full Chlamy only time series data.
</commit_message>
<xml_diff>
--- a/pilot-projects/07_full_pilot_plate_design.xlsx
+++ b/pilot-projects/07_full_pilot_plate_design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bbf9a23e224bd51a/Documents/GitHub/Chlamydomonas_mic_JRL_2024/pilot-projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="390" documentId="8_{10A8A257-CE5D-4C81-A3C8-11AF84C3F4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEDC1581-4E29-4DF7-844A-82ACECB1190A}"/>
+  <xr:revisionPtr revIDLastSave="404" documentId="8_{10A8A257-CE5D-4C81-A3C8-11AF84C3F4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2B549F0-B68C-477F-8A83-BEF005C2856E}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="9" xr2:uid="{994FF239-CC52-48A6-8C06-6EDEC1475B1C}"/>
   </bookViews>
@@ -262,15 +262,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -281,6 +272,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -300,6 +300,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -622,7 +626,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18:M19"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +664,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -668,26 +672,26 @@
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6">
-        <v>4</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -696,20 +700,20 @@
         <v>8</v>
       </c>
       <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
+        <v>2</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -718,35 +722,35 @@
         <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="1">
-        <v>2</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="E5" s="3">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -765,23 +769,23 @@
       <c r="E6" s="1">
         <v>5</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
@@ -790,23 +794,23 @@
         <v>7</v>
       </c>
       <c r="E7" s="1">
-        <v>8</v>
-      </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
@@ -815,32 +819,32 @@
         <v>7</v>
       </c>
       <c r="E8" s="1">
-        <v>9</v>
-      </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -848,7 +852,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>7</v>
@@ -857,7 +861,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G10" s="1">
         <f>43/3</f>
@@ -867,14 +871,14 @@
         <f>G10*9</f>
         <v>129</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G12" s="1">
@@ -885,29 +889,29 @@
         <f>G12*3</f>
         <v>32</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+      <c r="A13" s="2"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G15" s="1" t="s">
@@ -928,13 +932,13 @@
         <f>G18*3</f>
         <v>99</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="I18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
     </row>
     <row r="19" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G19" s="1">
@@ -945,11 +949,11 @@
         <f>G19*3</f>
         <v>93</v>
       </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
     </row>
     <row r="21" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G21" s="1">
@@ -962,9 +966,12 @@
       </c>
     </row>
     <row r="24" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G24" s="5"/>
+      <c r="G24" s="2"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E24">
+    <sortCondition ref="E2:E24"/>
+  </sortState>
   <mergeCells count="6">
     <mergeCell ref="I18:M19"/>
     <mergeCell ref="G2:N4"/>
@@ -982,7 +989,7 @@
   <dimension ref="A1:R172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection sqref="A1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,19 +1088,19 @@
       <c r="H3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="5">
-        <v>2</v>
-      </c>
-      <c r="K3" s="4" t="s">
+      <c r="I3" s="2">
+        <v>2</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -1123,14 +1130,14 @@
       <c r="I4">
         <v>3</v>
       </c>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -1160,14 +1167,14 @@
       <c r="I5">
         <v>4</v>
       </c>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -1226,16 +1233,16 @@
       <c r="I7">
         <v>6</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -1265,14 +1272,14 @@
       <c r="I8">
         <v>7</v>
       </c>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -1302,14 +1309,14 @@
       <c r="I9">
         <v>8</v>
       </c>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -1380,12 +1387,12 @@
         <f>L11-96</f>
         <v>75</v>
       </c>
-      <c r="O11" s="2" t="s">
+      <c r="O11" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -1444,16 +1451,16 @@
       <c r="I13">
         <v>12</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="K13" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -1483,14 +1490,14 @@
       <c r="I14">
         <v>13</v>
       </c>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -1520,14 +1527,14 @@
       <c r="I15">
         <v>14</v>
       </c>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -1554,7 +1561,7 @@
       <c r="H16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I16" s="2">
         <v>15</v>
       </c>
     </row>
@@ -1598,39 +1605,39 @@
         <f>L17/96</f>
         <v>25.53125</v>
       </c>
-      <c r="O17" s="2" t="s">
+      <c r="O17" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18" s="9">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="B18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="1">
-        <v>3</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I18">
+      <c r="D18" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="9">
+        <v>3</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="10">
         <v>17</v>
       </c>
     </row>
@@ -1638,28 +1645,28 @@
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="9" t="s">
+      <c r="B19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" s="9">
-        <v>1</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I19" s="10">
+      <c r="E19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19">
         <v>18</v>
       </c>
       <c r="K19">
@@ -1674,12 +1681,12 @@
         <f>L19/96</f>
         <v>18.40625</v>
       </c>
-      <c r="O19" s="2" t="s">
+      <c r="O19" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -1767,7 +1774,7 @@
       <c r="I22">
         <v>21</v>
       </c>
-      <c r="J22" s="5"/>
+      <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -2319,7 +2326,7 @@
       <c r="I41">
         <v>40</v>
       </c>
-      <c r="K41" s="5"/>
+      <c r="K41" s="2"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
@@ -3393,7 +3400,7 @@
       <c r="I78">
         <v>77</v>
       </c>
-      <c r="K78" s="5"/>
+      <c r="K78" s="2"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
@@ -3797,7 +3804,7 @@
       <c r="H92" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I92" s="5">
+      <c r="I92" s="2">
         <v>91</v>
       </c>
     </row>
@@ -3946,36 +3953,36 @@
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="7">
-        <v>1</v>
-      </c>
-      <c r="B98" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C98" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D98" s="7" t="s">
+    <row r="98" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="4">
+        <v>1</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D98" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E98" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F98" s="7">
-        <v>1</v>
-      </c>
-      <c r="G98" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H98" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I98" s="8">
+      <c r="E98" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F98" s="4">
+        <v>1</v>
+      </c>
+      <c r="G98" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H98" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I98" s="5">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>2</v>
       </c>
@@ -4551,10 +4558,10 @@
       <c r="H118" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I118" s="5">
+      <c r="I118" s="2">
         <v>117</v>
       </c>
-      <c r="M118" s="5"/>
+      <c r="M118" s="2"/>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
@@ -4995,25 +5002,25 @@
       <c r="A134" s="1">
         <v>37</v>
       </c>
-      <c r="B134" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C134" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D134" s="9" t="s">
+      <c r="B134" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D134" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E134" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F134" s="9">
-        <v>2</v>
-      </c>
-      <c r="G134" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H134" s="9" t="s">
+      <c r="E134" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F134" s="1">
+        <v>2</v>
+      </c>
+      <c r="G134" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H134" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I134">
@@ -5108,31 +5115,31 @@
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A138" s="1">
+      <c r="A138" s="9">
         <v>41</v>
       </c>
-      <c r="B138" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C138" s="1" t="s">
+      <c r="B138" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C138" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D138" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E138" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F138" s="1">
-        <v>2</v>
-      </c>
-      <c r="G138" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H138" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I138">
+      <c r="D138" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E138" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F138" s="9">
+        <v>2</v>
+      </c>
+      <c r="G138" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H138" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I138" s="10">
         <v>137</v>
       </c>
     </row>
@@ -5512,7 +5519,7 @@
       <c r="I151">
         <v>150</v>
       </c>
-      <c r="K151" s="5"/>
+      <c r="K151" s="2"/>
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
@@ -5916,7 +5923,7 @@
       <c r="H165" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I165" s="5">
+      <c r="I165" s="2">
         <v>164</v>
       </c>
     </row>
@@ -6124,16 +6131,16 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:I172">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I172">
     <sortCondition ref="I2:I172"/>
   </sortState>
   <mergeCells count="6">
+    <mergeCell ref="O19:R19"/>
     <mergeCell ref="K3:R5"/>
     <mergeCell ref="K7:R9"/>
     <mergeCell ref="O11:R11"/>
     <mergeCell ref="K13:R15"/>
     <mergeCell ref="O17:R17"/>
-    <mergeCell ref="O19:R19"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6145,7 +6152,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6187,77 +6194,77 @@
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6">
-        <v>1</v>
-      </c>
-      <c r="F2" s="5"/>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="1">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -6279,41 +6286,41 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E8" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1">
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1">
         <v>3</v>
@@ -6322,16 +6329,19 @@
         <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E10" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+      <c r="A13" s="2"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E13">
+    <sortCondition ref="E2:E13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6341,7 +6351,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6375,7 +6385,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -6383,25 +6393,25 @@
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6">
-        <v>3</v>
+      <c r="E2" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -6409,7 +6419,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -6417,26 +6427,26 @@
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="G4" s="5"/>
+      <c r="E4" s="3">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -6444,7 +6454,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>8</v>
@@ -6453,7 +6463,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -6478,7 +6488,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
@@ -6487,7 +6497,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -6495,7 +6505,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>7</v>
@@ -6504,30 +6514,33 @@
         <v>7</v>
       </c>
       <c r="E9" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E10" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+      <c r="A13" s="2"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E13">
+    <sortCondition ref="E2:E13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6537,7 +6550,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection sqref="A1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6568,7 +6581,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -6577,12 +6590,12 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="6">
-        <v>3</v>
-      </c>
-      <c r="H2" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -6606,7 +6619,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -6614,42 +6627,42 @@
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1">
-        <v>4</v>
+      <c r="E4" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -6657,7 +6670,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
@@ -6666,7 +6679,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -6674,7 +6687,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
@@ -6683,47 +6696,50 @@
         <v>7</v>
       </c>
       <c r="E8" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1">
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1">
         <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+      <c r="A13" s="2"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E13">
+    <sortCondition ref="E2:E13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6733,7 +6749,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6767,7 +6783,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -6775,77 +6791,77 @@
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6">
-        <v>8</v>
+      <c r="E2" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -6853,7 +6869,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
@@ -6862,41 +6878,41 @@
         <v>7</v>
       </c>
       <c r="E7" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="1">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="E9" s="3">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -6917,9 +6933,12 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+      <c r="A13" s="2"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E13">
+    <sortCondition ref="E2:E13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6929,7 +6948,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6961,28 +6980,28 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="6">
-        <v>2</v>
-      </c>
-      <c r="H2" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -6990,25 +7009,25 @@
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1">
-        <v>7</v>
+      <c r="E3" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -7016,7 +7035,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
@@ -7025,7 +7044,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -7033,7 +7052,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>8</v>
@@ -7042,41 +7061,41 @@
         <v>7</v>
       </c>
       <c r="E6" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E8" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -7084,7 +7103,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>7</v>
@@ -7093,7 +7112,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -7101,7 +7120,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>7</v>
@@ -7110,13 +7129,16 @@
         <v>7</v>
       </c>
       <c r="E10" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+      <c r="A13" s="2"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E13">
+    <sortCondition ref="E2:E13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7126,7 +7148,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection sqref="A1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7168,60 +7190,60 @@
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6">
-        <v>1</v>
-      </c>
-      <c r="H2" s="5"/>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -7243,36 +7265,36 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -7280,7 +7302,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>7</v>
@@ -7289,30 +7311,33 @@
         <v>7</v>
       </c>
       <c r="E9" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1">
         <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+      <c r="A13" s="2"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E13">
+    <sortCondition ref="E2:E13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7322,7 +7347,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection sqref="A1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7353,19 +7378,19 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="6">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -7373,7 +7398,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -7382,59 +7407,59 @@
         <v>8</v>
       </c>
       <c r="E3" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1">
-        <v>3</v>
-      </c>
-      <c r="H5" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -7459,7 +7484,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
@@ -7468,24 +7493,24 @@
         <v>7</v>
       </c>
       <c r="E8" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="1">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="E9" s="3">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -7493,7 +7518,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>7</v>
@@ -7502,13 +7527,16 @@
         <v>7</v>
       </c>
       <c r="E10" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+      <c r="A13" s="2"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E13">
+    <sortCondition ref="E2:E13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7560,42 +7588,42 @@
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -7617,54 +7645,54 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1">
-        <v>7</v>
-      </c>
-      <c r="L6" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -7672,7 +7700,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>7</v>
@@ -7681,7 +7709,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -7689,7 +7717,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>7</v>
@@ -7698,13 +7726,16 @@
         <v>7</v>
       </c>
       <c r="E10" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+      <c r="A13" s="2"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E13">
+    <sortCondition ref="E2:E13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Em1022 x Chlamy pilot project files
Raw output (RFUs, ODs) in tables
</commit_message>
<xml_diff>
--- a/pilot-projects/07_full_pilot_plate_design.xlsx
+++ b/pilot-projects/07_full_pilot_plate_design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bbf9a23e224bd51a/Documents/GitHub/Chlamydomonas_mic_JRL_2024/pilot-projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="404" documentId="8_{10A8A257-CE5D-4C81-A3C8-11AF84C3F4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2B549F0-B68C-477F-8A83-BEF005C2856E}"/>
+  <xr:revisionPtr revIDLastSave="406" documentId="8_{10A8A257-CE5D-4C81-A3C8-11AF84C3F4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73737D11-FE6E-4A63-97A9-37D6BE60C743}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="9" xr2:uid="{994FF239-CC52-48A6-8C06-6EDEC1475B1C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="9" xr2:uid="{994FF239-CC52-48A6-8C06-6EDEC1475B1C}"/>
   </bookViews>
   <sheets>
     <sheet name="8C" sheetId="1" r:id="rId1"/>
@@ -989,7 +989,7 @@
   <dimension ref="A1:R172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1048576"/>
+      <selection activeCell="B1" sqref="B1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1613,31 +1613,31 @@
       <c r="R17" s="8"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="9" t="s">
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="9">
-        <v>3</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I18" s="10">
+      <c r="D18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="1">
+        <v>3</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18">
         <v>17</v>
       </c>
     </row>
@@ -3376,28 +3376,28 @@
       <c r="A78" s="1">
         <v>77</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D78" s="1" t="s">
+      <c r="B78" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D78" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E78" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F78" s="1">
-        <v>2</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H78" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I78">
+      <c r="E78" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F78" s="9">
+        <v>2</v>
+      </c>
+      <c r="G78" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H78" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I78" s="10">
         <v>77</v>
       </c>
       <c r="K78" s="2"/>
@@ -5115,31 +5115,31 @@
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A138" s="9">
+      <c r="A138" s="1">
         <v>41</v>
       </c>
-      <c r="B138" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C138" s="9" t="s">
+      <c r="B138" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C138" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D138" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E138" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F138" s="9">
-        <v>2</v>
-      </c>
-      <c r="G138" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H138" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="I138" s="10">
+      <c r="D138" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F138" s="1">
+        <v>2</v>
+      </c>
+      <c r="G138" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H138" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I138">
         <v>137</v>
       </c>
     </row>
@@ -6131,7 +6131,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I172">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:I172">
     <sortCondition ref="I2:I172"/>
   </sortState>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Worked on uploading and cleaning the raw plate reader data
Fixed few nomenclature issues (jl_1_35...) didn't have a C, wrote a script to process each temperature in loop. Working on data analysis now!
</commit_message>
<xml_diff>
--- a/pilot-projects/07_full_pilot_plate_design.xlsx
+++ b/pilot-projects/07_full_pilot_plate_design.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bbf9a23e224bd51a/Documents/GitHub/Chlamydomonas_mic_JRL_2024/pilot-projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="406" documentId="8_{10A8A257-CE5D-4C81-A3C8-11AF84C3F4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73737D11-FE6E-4A63-97A9-37D6BE60C743}"/>
+  <xr:revisionPtr revIDLastSave="408" documentId="8_{10A8A257-CE5D-4C81-A3C8-11AF84C3F4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CD34401-AEC4-4778-950B-FE4059B05623}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="9" xr2:uid="{994FF239-CC52-48A6-8C06-6EDEC1475B1C}"/>
   </bookViews>
@@ -257,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -281,10 +281,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,7 +622,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF7FD6D9-17A1-4D5A-B8DB-8642505DC544}">
   <dimension ref="A1:R172"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:I1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:H172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3376,28 +3372,28 @@
       <c r="A78" s="1">
         <v>77</v>
       </c>
-      <c r="B78" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C78" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D78" s="9" t="s">
+      <c r="B78" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E78" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F78" s="9">
-        <v>2</v>
-      </c>
-      <c r="G78" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H78" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I78" s="10">
+      <c r="E78" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F78" s="1">
+        <v>2</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I78">
         <v>77</v>
       </c>
       <c r="K78" s="2"/>
@@ -6152,7 +6148,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C2" sqref="C2:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6351,7 +6347,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C2" sqref="C2:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6550,7 +6546,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1048576"/>
+      <selection activeCell="C2" sqref="C2:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6749,7 +6745,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C2" sqref="C2:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6948,7 +6944,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="C2" sqref="C2:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7148,7 +7144,206 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1048576"/>
+      <selection activeCell="D2" sqref="C2:D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="10.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E13">
+    <sortCondition ref="E2:E13"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D587F10-E877-44B5-9361-7C9AC2BA327C}">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7179,205 +7374,6 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="3">
-        <v>1</v>
-      </c>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1">
-        <v>3</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="1">
-        <v>3</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E13">
-    <sortCondition ref="E2:E13"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D587F10-E877-44B5-9361-7C9AC2BA327C}">
-  <dimension ref="A1:H13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="10.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="11.28515625" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1">
@@ -7546,7 +7542,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1048576"/>
+      <selection activeCell="C2" sqref="C2:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>